<commit_message>
correct legend category B/C
</commit_message>
<xml_diff>
--- a/Data/TABLE S1_COM1.xlsx
+++ b/Data/TABLE S1_COM1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriehofstetter/Desktop/SOUR ROT SUBMISSION/FINAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriehofstetter/Desktop/SOUR ROT RESUBMISSION/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB241F9-FE19-D24F-9B41-662AE8D532B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EAC5BD8-2278-4740-9C2B-8E0B3BCC498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2620" yWindow="720" windowWidth="27660" windowHeight="18760" xr2:uid="{89A25F2E-5CBE-B84E-9E40-85B2FEE01AB5}"/>
   </bookViews>
@@ -926,6 +926,379 @@
   <si>
     <r>
       <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Penicillium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Penicillium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. 1</t>
+    </r>
+  </si>
+  <si>
+    <t>NR_077153, OQ870786 type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Geotrichum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Geotrichum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sp. 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pantoea </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">cf. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>agglomerans</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pantoea </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">cf. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">agglomerans </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>PQ104896</t>
+  </si>
+  <si>
+    <t>PQ104897</t>
+  </si>
+  <si>
+    <t>PQ104898</t>
+  </si>
+  <si>
+    <t>PQ104899</t>
+  </si>
+  <si>
+    <t>PQ114293</t>
+  </si>
+  <si>
+    <t>PQ114294</t>
+  </si>
+  <si>
+    <t>PQ114295</t>
+  </si>
+  <si>
+    <t>PQ114296</t>
+  </si>
+  <si>
+    <t>PQ114297</t>
+  </si>
+  <si>
+    <t>PQ114298</t>
+  </si>
+  <si>
+    <t>PQ114299</t>
+  </si>
+  <si>
+    <t>PQ114300</t>
+  </si>
+  <si>
+    <t>PQ114301</t>
+  </si>
+  <si>
+    <t>PQ114302</t>
+  </si>
+  <si>
+    <t>PQ114303</t>
+  </si>
+  <si>
+    <t>PQ114304</t>
+  </si>
+  <si>
+    <t>PQ114305</t>
+  </si>
+  <si>
+    <t>PQ114306</t>
+  </si>
+  <si>
+    <t>PQ114307</t>
+  </si>
+  <si>
+    <t>PQ114308</t>
+  </si>
+  <si>
+    <t>PQ114309</t>
+  </si>
+  <si>
+    <t>PQ114310</t>
+  </si>
+  <si>
+    <t>PQ114311</t>
+  </si>
+  <si>
+    <t>PQ114312</t>
+  </si>
+  <si>
+    <t>PQ114313</t>
+  </si>
+  <si>
+    <t>PQ114314</t>
+  </si>
+  <si>
+    <t>PQ114315</t>
+  </si>
+  <si>
+    <t>PQ114316</t>
+  </si>
+  <si>
+    <t>PQ114317</t>
+  </si>
+  <si>
+    <t>PQ114318</t>
+  </si>
+  <si>
+    <t>PQ114319</t>
+  </si>
+  <si>
+    <t>PQ114320</t>
+  </si>
+  <si>
+    <t>PQ114321</t>
+  </si>
+  <si>
+    <t>PQ114322</t>
+  </si>
+  <si>
+    <t>PQ114323</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mucor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> cf. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">circinelloides </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">f. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>circinelloides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mucor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> cf. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>circinelloides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> f. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>circinelloides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <b/>
         <sz val="12"/>
         <color theme="1"/>
@@ -941,380 +1314,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">. Voucher information for fungal and bacterial isolates. Bacteria are highlighted in green. A. Fungi isolated from sour rot symptomatic clusters of several cultivars harvested in Grisons , B. Bacteria and fungi isolated from sour rot symptomatic clusters harvested in Vaud (Nyon), C. Bacteria and fungi isolated from sour rot symptomatic clusters harvested in the canton of Vaud (Nyon), D. Bacteria and fungi isolated from grey mould symptomatic clusters harvested in the canton of Vaud (Nyon). Sequence alignment was carried out by grouping isolates from the experiments 1 and 2 (see materials and methods section and Table S2). Where ITS genotypes were identical in both experiments, we chose a single isolate from either experiment to perform sequence similarity searches in GenBank. Current names of the bacteria and fungi were obtained from LPSN (https://www.bacterio.net) and Mycobank (MB: https://www.mycobank.org)/Index Fungorum (IF: https://www.indexfungorum.org/Names/Names.asp) respectively. Searches for sequence similarity in GenBank and taxon current name have been conducted from March to Mai 2023. Where Mycobank and Index Fungorum indicated that the current name was not the one associated with the BLAST top score sequence or where the two databases disagred on the current name, we reported the correct or second name in parentheses. When type sequences where not flagged with NR_ in GenBank, we precised when they were type sequences. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Penicillium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sp. 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Penicillium</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sp. 1</t>
-    </r>
-  </si>
-  <si>
-    <t>NR_077153, OQ870786 type</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Geotrichum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sp. 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Geotrichum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> sp. 2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Pantoea </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">cf. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>agglomerans</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Pantoea </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">cf. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">agglomerans </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>PQ104896</t>
-  </si>
-  <si>
-    <t>PQ104897</t>
-  </si>
-  <si>
-    <t>PQ104898</t>
-  </si>
-  <si>
-    <t>PQ104899</t>
-  </si>
-  <si>
-    <t>PQ114293</t>
-  </si>
-  <si>
-    <t>PQ114294</t>
-  </si>
-  <si>
-    <t>PQ114295</t>
-  </si>
-  <si>
-    <t>PQ114296</t>
-  </si>
-  <si>
-    <t>PQ114297</t>
-  </si>
-  <si>
-    <t>PQ114298</t>
-  </si>
-  <si>
-    <t>PQ114299</t>
-  </si>
-  <si>
-    <t>PQ114300</t>
-  </si>
-  <si>
-    <t>PQ114301</t>
-  </si>
-  <si>
-    <t>PQ114302</t>
-  </si>
-  <si>
-    <t>PQ114303</t>
-  </si>
-  <si>
-    <t>PQ114304</t>
-  </si>
-  <si>
-    <t>PQ114305</t>
-  </si>
-  <si>
-    <t>PQ114306</t>
-  </si>
-  <si>
-    <t>PQ114307</t>
-  </si>
-  <si>
-    <t>PQ114308</t>
-  </si>
-  <si>
-    <t>PQ114309</t>
-  </si>
-  <si>
-    <t>PQ114310</t>
-  </si>
-  <si>
-    <t>PQ114311</t>
-  </si>
-  <si>
-    <t>PQ114312</t>
-  </si>
-  <si>
-    <t>PQ114313</t>
-  </si>
-  <si>
-    <t>PQ114314</t>
-  </si>
-  <si>
-    <t>PQ114315</t>
-  </si>
-  <si>
-    <t>PQ114316</t>
-  </si>
-  <si>
-    <t>PQ114317</t>
-  </si>
-  <si>
-    <t>PQ114318</t>
-  </si>
-  <si>
-    <t>PQ114319</t>
-  </si>
-  <si>
-    <t>PQ114320</t>
-  </si>
-  <si>
-    <t>PQ114321</t>
-  </si>
-  <si>
-    <t>PQ114322</t>
-  </si>
-  <si>
-    <t>PQ114323</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Mucor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> cf. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">circinelloides </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">f. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>circinelloides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Mucor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> cf. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>circinelloides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> f. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>circinelloides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 2</t>
+      <t xml:space="preserve">. Voucher information for fungal and bacterial isolates. Bacteria are highlighted in green. A. Fungi isolated from sour rot symptomatic clusters of several cultivars harvested in Grisons , B. Bacteria and fungi isolated from sour rot symptomatic clusters of several cultivars harvested in Vaud, C. Bacteria and fungi isolated from sour rot symptomatic clusters harvested in a single vineyard plot at Nyon (Vaud), D. Bacteria and fungi isolated from grey mould symptomatic clusters harvested in a single vineyard plot at Nyon (Vaud). Sequence alignment was carried out by grouping isolates from the experiments 1 and 2 (see materials and methods section and Table S2). Where ITS genotypes were identical in both experiments, we chose a single isolate from either experiment to perform sequence similarity searches in GenBank. Current names of the bacteria and fungi were obtained from LPSN (https://www.bacterio.net) and Mycobank (MB: https://www.mycobank.org)/Index Fungorum (IF: https://www.indexfungorum.org/Names/Names.asp) respectively. Searches for sequence similarity in GenBank and taxon current name have been conducted from March to Mai 2023. Where Mycobank and Index Fungorum indicated that the current name was not the one associated with the BLAST top score sequence or where the two databases disagred on the current name, we reported the correct or second name in parentheses. When type sequences where not flagged with NR_ in GenBank, we precised when they were type sequences. </t>
     </r>
   </si>
 </sst>
@@ -1931,7 +1931,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -2001,7 +2001,7 @@
         <v>99</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>98</v>
@@ -2031,7 +2031,7 @@
         <v>102</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>100</v>
@@ -2060,7 +2060,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>68</v>
@@ -2089,7 +2089,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>69</v>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>133</v>
@@ -2151,7 +2151,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>70</v>
@@ -2180,7 +2180,7 @@
         <v>29</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>71</v>
@@ -2209,7 +2209,7 @@
         <v>31</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>72</v>
@@ -2238,7 +2238,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>74</v>
@@ -2273,7 +2273,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>73</v>
@@ -2306,7 +2306,7 @@
         <v>34</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I13" s="13" t="s">
         <v>75</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="22">
         <v>1</v>
@@ -2338,7 +2338,7 @@
         <v>35</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>76</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="22">
         <v>1</v>
@@ -2368,7 +2368,7 @@
         <v>36</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>77</v>
@@ -2398,7 +2398,7 @@
         <v>37</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>78</v>
@@ -2427,7 +2427,7 @@
         <v>39</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>79</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" s="22">
         <v>1</v>
@@ -2460,7 +2460,7 @@
         <v>41</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>80</v>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="19" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="21">
         <v>1</v>
@@ -2489,7 +2489,7 @@
         <v>42</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>80</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E20" s="20">
         <v>1</v>
@@ -2518,7 +2518,7 @@
         <v>107</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>108</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E21" s="20">
         <v>1</v>
@@ -2547,7 +2547,7 @@
         <v>110</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>112</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" s="22">
         <v>1</v>
@@ -2585,10 +2585,10 @@
         <v>43</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J22" s="18">
         <v>100</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="23" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" s="19"/>
       <c r="E23" s="21">
@@ -2615,7 +2615,7 @@
         <v>44</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>81</v>
@@ -2644,7 +2644,7 @@
         <v>46</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>82</v>
@@ -2673,7 +2673,7 @@
         <v>48</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>85</v>
@@ -2706,7 +2706,7 @@
         <v>49</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>85</v>
@@ -2736,7 +2736,7 @@
         <v>50</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>86</v>
@@ -2765,7 +2765,7 @@
         <v>53</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>87</v>
@@ -2795,7 +2795,7 @@
         <v>54</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>87</v>
@@ -2825,7 +2825,7 @@
         <v>55</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>87</v>
@@ -2858,7 +2858,7 @@
         <v>57</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>88</v>
@@ -2891,7 +2891,7 @@
         <v>59</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>89</v>
@@ -2924,7 +2924,7 @@
         <v>60</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>89</v>
@@ -2957,7 +2957,7 @@
         <v>61</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>89</v>
@@ -2987,7 +2987,7 @@
         <v>62</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>89</v>
@@ -3017,7 +3017,7 @@
         <v>64</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I36" s="13" t="s">
         <v>90</v>
@@ -3052,7 +3052,7 @@
         <v>66</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>91</v>

</xml_diff>